<commit_message>
Added types, effectiveness and moves Made weapon generator Created basic navigation object Basic CSS General high level divs
</commit_message>
<xml_diff>
--- a/docs/Type Effectiveness Chart.xlsx
+++ b/docs/Type Effectiveness Chart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crispis.IGI\Documents\HoD V2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crispis.IGI\Documents\HoD V2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{98889683-DC4B-4D51-A2A6-FEF77A59AE1C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5AFE8F05-F44E-4432-9AC8-2A41B5D6EE9A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{A35E9858-D659-4FFF-8F07-35C1F4418800}"/>
   </bookViews>
@@ -87,8 +87,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -102,32 +105,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -455,26 +437,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D63AB1AC-9C9A-4F03-8A87-9957D8D9D9EB}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C1" s="2" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>2</v>
@@ -498,8 +480,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -524,19 +506,23 @@
         <v>1</v>
       </c>
       <c r="I3" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="J3">
+        <f>SUM(C3:I3)</f>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="1">
-        <v>1</v>
+      <c r="D4" s="2">
+        <v>0.5</v>
       </c>
       <c r="E4" s="1">
         <v>0.5</v>
@@ -551,11 +537,15 @@
         <v>2</v>
       </c>
       <c r="I4" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J9" si="0">SUM(C4:I4)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -565,8 +555,8 @@
       <c r="D5" s="1">
         <v>2</v>
       </c>
-      <c r="E5" s="1">
-        <v>1</v>
+      <c r="E5" s="2">
+        <v>0.5</v>
       </c>
       <c r="F5" s="1">
         <v>0.5</v>
@@ -578,11 +568,15 @@
         <v>2</v>
       </c>
       <c r="I5" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -595,8 +589,8 @@
       <c r="E6" s="1">
         <v>2</v>
       </c>
-      <c r="F6" s="1">
-        <v>1</v>
+      <c r="F6" s="2">
+        <v>0.5</v>
       </c>
       <c r="G6" s="1">
         <v>1</v>
@@ -605,11 +599,15 @@
         <v>1</v>
       </c>
       <c r="I6" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
@@ -632,11 +630,15 @@
         <v>0.5</v>
       </c>
       <c r="I7" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
@@ -655,38 +657,76 @@
       <c r="G8" s="1">
         <v>0.5</v>
       </c>
-      <c r="H8" s="1">
-        <v>1</v>
+      <c r="H8" s="2">
+        <v>0.5</v>
       </c>
       <c r="I8" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="1">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="D9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" s="1">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="F9" s="1">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="G9" s="1">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="H9" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I9" s="1">
-        <v>1</v>
+        <v>0.5</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <f>SUM(C3:C9)</f>
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ref="D10:I10" si="1">SUM(D3:D9)</f>
+        <v>6.5</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>6.5</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
       </c>
     </row>
   </sheetData>
@@ -695,13 +735,13 @@
     <mergeCell ref="A3:A9"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:I9">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="0.5">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="0.5">
       <formula>NOT(ISERROR(SEARCH("0.5",C3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="2">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="2">
       <formula>NOT(ISERROR(SEARCH("2",C3)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>